<commit_message>
include 13700T in CoreMark comparison graph
</commit_message>
<xml_diff>
--- a/CoreMark/CoreMark.xlsx
+++ b/CoreMark/CoreMark.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/Documents/GitHub/benchmark/CoreMark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DEC05-A86D-B640-BD69-18A7BFF966BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA5CA1B-D74C-B24E-9E05-F33C764EAD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="860" windowWidth="20520" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2023" sheetId="3" r:id="rId1"/>
+    <sheet name="2024" sheetId="3" r:id="rId1"/>
     <sheet name="multi" sheetId="2" r:id="rId2"/>
     <sheet name="single" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -255,18 +255,9 @@
     <t>Core Gen 10</t>
   </si>
   <si>
-    <t>i7-12700T</t>
-  </si>
-  <si>
-    <t>Core Gen 12</t>
-  </si>
-  <si>
     <t>note2</t>
   </si>
   <si>
-    <t>Alder Lake-S</t>
-  </si>
-  <si>
     <t>Firestorm</t>
   </si>
   <si>
@@ -274,6 +265,15 @@
   </si>
   <si>
     <t>plus undocumented AMX instr.</t>
+  </si>
+  <si>
+    <t>i7-13700T</t>
+  </si>
+  <si>
+    <t>Core Gen 13</t>
+  </si>
+  <si>
+    <t>Raptor Lake-S</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -660,7 +660,7 @@
     <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,7 +698,7 @@
         <v>51</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1159,20 +1159,29 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="B21">
+        <v>39082</v>
+      </c>
+      <c r="C21">
+        <v>4600</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4960869565217383</v>
+      </c>
       <c r="E21">
         <v>2024</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
         <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I21">
         <v>64</v>
@@ -1196,13 +1205,13 @@
         <v>2023</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I22">
         <v>64</v>
@@ -1223,6 +1232,7 @@
     <hyperlink ref="A28" r:id="rId1" xr:uid="{14E13CF2-D12C-470D-B931-64AFEE59DDEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
include G2030 and details for CPUs
</commit_message>
<xml_diff>
--- a/CoreMark/CoreMark.xlsx
+++ b/CoreMark/CoreMark.xlsx
@@ -1,40 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/Documents/GitHub/benchmark/CoreMark/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\benchmark\CoreMark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA5CA1B-D74C-B24E-9E05-F33C764EAD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3988876D-9068-437B-BF43-C5924FBE3AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="860" windowWidth="20520" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27660" yWindow="510" windowWidth="23910" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="3" r:id="rId1"/>
     <sheet name="multi" sheetId="2" r:id="rId2"/>
-    <sheet name="single" sheetId="1" r:id="rId3"/>
+    <sheet name="single2021" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>CoreMark Values</t>
   </si>
@@ -237,24 +225,12 @@
     <t>Ivy Bridge</t>
   </si>
   <si>
-    <t>Core Gen 3</t>
-  </si>
-  <si>
-    <t>Core Gen 6</t>
-  </si>
-  <si>
     <t>Skylake-H</t>
   </si>
   <si>
-    <t>Nehalem, Core Gen 1</t>
-  </si>
-  <si>
     <t>Comet Lake-S</t>
   </si>
   <si>
-    <t>Core Gen 10</t>
-  </si>
-  <si>
     <t>note2</t>
   </si>
   <si>
@@ -274,6 +250,45 @@
   </si>
   <si>
     <t>Raptor Lake-S</t>
+  </si>
+  <si>
+    <t>Pentium G2030</t>
+  </si>
+  <si>
+    <t>CoreMark Values - 2 threads</t>
+  </si>
+  <si>
+    <t>2 threads</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>LX7</t>
+  </si>
+  <si>
+    <t>LX6</t>
+  </si>
+  <si>
+    <t>Xtensa</t>
+  </si>
+  <si>
+    <t>Core Gen 3, Ivy Bridge 22nm</t>
+  </si>
+  <si>
+    <t>Core Gen 1, Nehalem 45nm</t>
+  </si>
+  <si>
+    <t>Core Gen 6, Skylake 14nm</t>
+  </si>
+  <si>
+    <t>Core Gen 10, Comet Lake 14 nm</t>
+  </si>
+  <si>
+    <t>RV32IMV</t>
+  </si>
+  <si>
+    <t>https://www.espressif.com/sites/default/files/documentation/esp32-c3_technical_reference_manual_en.pdf#riscvcpu</t>
   </si>
 </sst>
 </file>
@@ -645,591 +660,719 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9321212E-8ABB-4B14-AEF6-E9EC57B10669}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>38</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>46</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>48</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>51</v>
       </c>
-      <c r="J3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
+        <f>C4/D4</f>
+        <v>0.4375</v>
+      </c>
+      <c r="C4">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>16</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" ref="D4:D22" si="0">B4/C4</f>
-        <v>0.4375</v>
-      </c>
       <c r="E4">
+        <v>1997</v>
+      </c>
+      <c r="F4">
         <v>2020</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>57</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>58</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:B17" si="0">C5/D5</f>
+        <v>1.125</v>
+      </c>
+      <c r="C5">
         <v>81</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>72</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>1.125</v>
-      </c>
       <c r="E5">
+        <v>2007</v>
+      </c>
+      <c r="F5">
         <v>2020</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7857142857142858</v>
+      </c>
+      <c r="C6">
         <v>150</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>84</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7857142857142858</v>
-      </c>
       <c r="E6">
+        <v>2013</v>
+      </c>
+      <c r="F6">
         <v>2020</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>32</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
+      </c>
+      <c r="C7">
         <v>172</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>100</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.72</v>
-      </c>
       <c r="E7">
+        <v>2013</v>
+      </c>
+      <c r="F7">
         <v>2020</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>52</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>32</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.481203007518797</v>
+      </c>
+      <c r="C8">
         <v>197</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>133</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>1.481203007518797</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="E8">
+        <v>2021</v>
+      </c>
+      <c r="F8" s="3">
         <v>2023</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="C9">
         <v>304</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>160</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="E9">
+        <v>2016</v>
+      </c>
+      <c r="F9" s="3">
         <v>2023</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>56</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" t="s">
         <v>47</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1937500000000001</v>
+      </c>
+      <c r="C10">
         <v>351</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>160</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1937500000000001</v>
-      </c>
       <c r="E10">
+        <v>2016</v>
+      </c>
+      <c r="F10">
         <v>2020</v>
       </c>
-      <c r="I10">
+      <c r="H10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2562500000000001</v>
+      </c>
+      <c r="C11">
         <v>361</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>160</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2562500000000001</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="E11">
+        <v>2019</v>
+      </c>
+      <c r="F11" s="3">
         <v>2023</v>
       </c>
-      <c r="I11">
+      <c r="H11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.34375</v>
+      </c>
+      <c r="C12">
         <v>375</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>160</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>2.34375</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="E12">
+        <v>2016</v>
+      </c>
+      <c r="F12" s="3">
         <v>2023</v>
       </c>
-      <c r="I12">
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8791666666666667</v>
+      </c>
+      <c r="C13">
         <v>451</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>240</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>1.8791666666666667</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="E13">
+        <v>2020</v>
+      </c>
+      <c r="F13" s="3">
         <v>2023</v>
       </c>
-      <c r="I13">
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2485714285714287</v>
+      </c>
+      <c r="C14">
         <v>1574</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>700</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2485714285714287</v>
-      </c>
       <c r="E14">
+        <v>2012</v>
+      </c>
+      <c r="F14">
         <v>2020</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>60</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>59</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="C15">
         <v>3800</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>1200</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>3.1666666666666665</v>
-      </c>
       <c r="E15">
+        <v>2016</v>
+      </c>
+      <c r="F15">
         <v>2020</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>62</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>61</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2608333333333333</v>
+      </c>
+      <c r="C16">
         <v>3913</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>1200</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>3.2608333333333333</v>
-      </c>
       <c r="E16">
+        <v>2015</v>
+      </c>
+      <c r="F16">
         <v>2020</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>63</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>61</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4584967320261439</v>
+      </c>
+      <c r="C17">
         <v>13643</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>3060</v>
       </c>
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>4.4584967320261439</v>
-      </c>
       <c r="E17">
+        <v>2009</v>
+      </c>
+      <c r="F17">
         <v>2020</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1">
+        <f>C18/D18</f>
+        <v>6.3620000000000001</v>
+      </c>
+      <c r="C18">
+        <v>19086</v>
+      </c>
+      <c r="D18">
+        <v>3000</v>
+      </c>
+      <c r="E18">
+        <v>2013</v>
+      </c>
+      <c r="F18">
+        <v>2024</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" ref="B19:B23" si="1">C19/D19</f>
+        <v>6.4378787878787875</v>
+      </c>
+      <c r="C19">
+        <v>21245</v>
+      </c>
+      <c r="D19">
+        <v>3300</v>
+      </c>
+      <c r="E19">
+        <v>2012</v>
+      </c>
+      <c r="F19">
+        <v>2020</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4969945355191259</v>
+      </c>
+      <c r="C20">
+        <v>23779</v>
+      </c>
+      <c r="D20">
+        <v>3660</v>
+      </c>
+      <c r="E20">
+        <v>2015</v>
+      </c>
+      <c r="F20">
+        <v>2020</v>
+      </c>
+      <c r="G20" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>7.2350710900473931</v>
+      </c>
+      <c r="C21">
+        <v>30532</v>
+      </c>
+      <c r="D21">
+        <v>4220</v>
+      </c>
+      <c r="E21">
+        <v>2020</v>
+      </c>
+      <c r="F21">
+        <v>2021</v>
+      </c>
+      <c r="G21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4960869565217383</v>
+      </c>
+      <c r="C22">
+        <v>39082</v>
+      </c>
+      <c r="D22">
+        <v>4600</v>
+      </c>
+      <c r="E22">
+        <v>2023</v>
+      </c>
+      <c r="F22">
+        <v>2024</v>
+      </c>
+      <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="1"/>
+        <v>9.9118750000000002</v>
+      </c>
+      <c r="C23">
+        <v>31718</v>
+      </c>
+      <c r="D23">
+        <v>3200</v>
+      </c>
+      <c r="E23">
+        <v>2020</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2023</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" t="s">
         <v>70</v>
       </c>
-      <c r="G17" t="s">
+      <c r="J23">
         <v>64</v>
       </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>21245</v>
-      </c>
-      <c r="C18">
-        <v>3300</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>6.4378787878787875</v>
-      </c>
-      <c r="E18">
-        <v>2020</v>
-      </c>
-      <c r="F18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19">
-        <v>23779</v>
-      </c>
-      <c r="C19">
-        <v>3660</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>6.4969945355191259</v>
-      </c>
-      <c r="E19">
-        <v>2020</v>
-      </c>
-      <c r="F19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>30532</v>
-      </c>
-      <c r="C20">
-        <v>4220</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>7.2350710900473931</v>
-      </c>
-      <c r="E20">
-        <v>2021</v>
-      </c>
-      <c r="F20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21">
-        <v>39082</v>
-      </c>
-      <c r="C21">
-        <v>4600</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>8.4960869565217383</v>
-      </c>
-      <c r="E21">
-        <v>2024</v>
-      </c>
-      <c r="F21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22">
-        <v>31718</v>
-      </c>
-      <c r="C22">
-        <v>3200</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>9.9118750000000002</v>
-      </c>
-      <c r="E22" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F22" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B29" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A28" r:id="rId1" xr:uid="{14E13CF2-D12C-470D-B931-64AFEE59DDEB}"/>
+    <hyperlink ref="A29" r:id="rId1" xr:uid="{14E13CF2-D12C-470D-B931-64AFEE59DDEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1238,31 +1381,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978EF068-C664-40CD-A690-2ADA683B78C9}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1276,208 +1419,247 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>36943</v>
+      </c>
+      <c r="C4">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4/2</f>
+        <v>6.1571666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="B9">
         <v>15194</v>
       </c>
-      <c r="C4">
+      <c r="C9">
         <v>1200</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D9" s="1">
         <v>3.16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
+      <c r="B10">
         <v>15393</v>
       </c>
-      <c r="C5">
+      <c r="C10">
         <v>1200</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D10" s="1">
         <v>3.21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B11">
         <v>32880</v>
       </c>
-      <c r="C6">
+      <c r="C11">
         <v>1500</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D11" s="1">
         <v>5.48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B7">
+      <c r="B12">
         <v>53450</v>
       </c>
-      <c r="C7">
+      <c r="C12">
         <v>3300</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D12" s="1">
         <v>4.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B8">
+      <c r="B13">
         <v>74944</v>
       </c>
-      <c r="C8">
+      <c r="C13">
         <v>3800</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D13" s="1">
         <v>4.93</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
+      <c r="B14">
         <v>96420</v>
       </c>
-      <c r="C9">
+      <c r="C14">
         <v>3660</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D14" s="1">
         <v>6.7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B10">
+      <c r="B15">
         <v>103808</v>
       </c>
-      <c r="C10">
+      <c r="C15">
         <v>4070</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D15" s="1">
         <v>6.38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C20" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
+      <c r="B21">
         <v>95261</v>
       </c>
-      <c r="C16">
+      <c r="C21">
         <v>3800</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D21" s="1">
         <v>3.13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
+      <c r="B22">
         <v>118862</v>
       </c>
-      <c r="C17">
+      <c r="C22">
         <v>3660</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D22" s="1">
         <v>4.13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B18">
+      <c r="B23">
         <v>167829</v>
       </c>
-      <c r="C18">
+      <c r="C23">
         <v>4070</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D23" s="1">
         <v>4.95</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C30" t="s">
         <v>3</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B31">
         <v>124634</v>
       </c>
-      <c r="C26">
+      <c r="C31">
         <v>3060</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D31" s="1">
         <v>2.5499999999999998</v>
       </c>
     </row>
@@ -1492,214 +1674,214 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
+        <f>C4/D4</f>
+        <v>0.4375</v>
+      </c>
+      <c r="C4">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>16</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" ref="D4:D15" si="0">B4/C4</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:B15" si="0">C5/D5</f>
+        <v>1.125</v>
+      </c>
+      <c r="C5">
         <v>81</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>72</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>1.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7857142857142858</v>
+      </c>
+      <c r="C6">
         <v>150</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>84</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7857142857142858</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
+      </c>
+      <c r="C7">
         <v>172</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>100</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1937500000000001</v>
+      </c>
+      <c r="C8">
         <v>351</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>160</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1937500000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2485714285714287</v>
+      </c>
+      <c r="C9">
         <v>1574</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>700</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2485714285714287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="C10">
         <v>3800</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1200</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>3.1666666666666665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2608333333333333</v>
+      </c>
+      <c r="C11">
         <v>3913</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1200</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>3.2608333333333333</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4584967320261439</v>
+      </c>
+      <c r="C12">
         <v>13643</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>3060</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>4.4584967320261439</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>6.4378787878787875</v>
+      </c>
+      <c r="C13">
         <v>21245</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>3300</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>6.4378787878787875</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>6.4969945355191259</v>
+      </c>
+      <c r="C14">
         <v>23779</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>3660</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>6.4969945355191259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2350710900473931</v>
+      </c>
+      <c r="C15">
         <v>30532</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>4220</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>7.2350710900473931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025 update on results, newly ordered
</commit_message>
<xml_diff>
--- a/CoreMark/CoreMark.xlsx
+++ b/CoreMark/CoreMark.xlsx
@@ -1,28 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\benchmark\CoreMark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archive\github\benchmark\CoreMark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3988876D-9068-437B-BF43-C5924FBE3AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1436DA8-C66D-41A0-A8DE-4BEEFEAB1B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27660" yWindow="510" windowWidth="23910" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29025" yWindow="255" windowWidth="21150" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024" sheetId="3" r:id="rId1"/>
+    <sheet name="2025" sheetId="3" r:id="rId1"/>
     <sheet name="multi" sheetId="2" r:id="rId2"/>
     <sheet name="single2021" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
   <si>
     <t>CoreMark Values</t>
   </si>
@@ -261,9 +272,6 @@
     <t>2 threads</t>
   </si>
   <si>
-    <t>build</t>
-  </si>
-  <si>
     <t>LX7</t>
   </si>
   <si>
@@ -289,13 +297,58 @@
   </si>
   <si>
     <t>https://www.espressif.com/sites/default/files/documentation/esp32-c3_technical_reference_manual_en.pdf#riscvcpu</t>
+  </si>
+  <si>
+    <t>RockChip 3229</t>
+  </si>
+  <si>
+    <t>Cortex A7</t>
+  </si>
+  <si>
+    <t>would be Raspberry Pi 2</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4 v1.1 4GB</t>
+  </si>
+  <si>
+    <t>ARMv7-A</t>
+  </si>
+  <si>
+    <t>Cortex-A72</t>
+  </si>
+  <si>
+    <t>announced 2015</t>
+  </si>
+  <si>
+    <t>announced 2012</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>CM/MHz</t>
+  </si>
+  <si>
+    <t>theory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +364,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,8 +386,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -334,24 +407,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -364,7 +484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -660,102 +780,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9321212E-8ABB-4B14-AEF6-E9EC57B10669}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.42578125" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N2" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="15">
         <f>C4/D4</f>
         <v>0.4375</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="14">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="14">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="14">
+        <v>8</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14">
         <v>1997</v>
       </c>
-      <c r="F4">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="14">
         <v>2020</v>
       </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ref="B5:B17" si="0">C5/D5</f>
+        <f t="shared" ref="B5:B19" si="0">C5/D5</f>
         <v>1.125</v>
       </c>
       <c r="C5">
@@ -764,23 +909,23 @@
       <c r="D5">
         <v>72</v>
       </c>
-      <c r="E5">
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5">
+        <v>32</v>
+      </c>
+      <c r="J5">
         <v>2007</v>
       </c>
-      <c r="F5">
+      <c r="O5">
         <v>2020</v>
       </c>
-      <c r="H5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -794,26 +939,26 @@
       <c r="D6">
         <v>84</v>
       </c>
-      <c r="E6">
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6">
+        <v>32</v>
+      </c>
+      <c r="J6">
         <v>2013</v>
       </c>
-      <c r="F6">
+      <c r="M6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6">
         <v>2020</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6">
-        <v>32</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -827,27 +972,27 @@
       <c r="D7">
         <v>100</v>
       </c>
-      <c r="E7">
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7">
+        <v>32</v>
+      </c>
+      <c r="J7">
         <v>2013</v>
       </c>
-      <c r="F7">
+      <c r="M7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7">
         <v>2020</v>
       </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7">
-        <v>32</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="1">
@@ -860,26 +1005,29 @@
       <c r="D8">
         <v>133</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8">
+        <v>32</v>
+      </c>
+      <c r="J8">
         <v>2021</v>
       </c>
-      <c r="F8" s="3">
+      <c r="N8" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="O8" s="3">
         <v>2023</v>
       </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -893,29 +1041,29 @@
       <c r="D9">
         <v>160</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9">
+        <v>32</v>
+      </c>
+      <c r="J9">
         <v>2016</v>
       </c>
-      <c r="F9" s="3">
+      <c r="M9" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="3">
         <v>2023</v>
       </c>
-      <c r="G9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9">
-        <v>32</v>
-      </c>
-      <c r="K9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -929,23 +1077,26 @@
       <c r="D10">
         <v>160</v>
       </c>
-      <c r="E10">
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>32</v>
+      </c>
+      <c r="J10">
         <v>2016</v>
       </c>
-      <c r="F10">
+      <c r="N10" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="O10">
         <v>2020</v>
       </c>
-      <c r="H10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -959,23 +1110,26 @@
       <c r="D11">
         <v>160</v>
       </c>
-      <c r="E11">
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11">
+        <v>32</v>
+      </c>
+      <c r="J11">
         <v>2019</v>
       </c>
-      <c r="F11" s="3">
+      <c r="N11" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="O11" s="3">
         <v>2023</v>
       </c>
-      <c r="H11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -989,23 +1143,26 @@
       <c r="D12">
         <v>160</v>
       </c>
-      <c r="E12">
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12">
+        <v>32</v>
+      </c>
+      <c r="J12">
         <v>2016</v>
       </c>
-      <c r="F12" s="3">
+      <c r="N12" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="O12" s="3">
         <v>2023</v>
       </c>
-      <c r="H12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I12" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1019,27 +1176,30 @@
       <c r="D13">
         <v>240</v>
       </c>
-      <c r="E13">
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13">
+        <v>32</v>
+      </c>
+      <c r="J13">
         <v>2020</v>
       </c>
-      <c r="F13" s="3">
+      <c r="M13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="O13" s="3">
         <v>2023</v>
       </c>
-      <c r="H13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13">
-        <v>32</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1">
@@ -1052,330 +1212,445 @@
       <c r="D14">
         <v>700</v>
       </c>
-      <c r="E14">
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14">
+        <v>32</v>
+      </c>
+      <c r="J14">
         <v>2012</v>
       </c>
-      <c r="F14">
+      <c r="N14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O14">
         <v>2020</v>
       </c>
-      <c r="H14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8436154949784793</v>
+      </c>
+      <c r="C15">
+        <v>3964</v>
+      </c>
+      <c r="D15">
+        <v>1394</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J15">
+        <v>2018</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="11">
         <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="12">
         <v>3800</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="12">
         <v>1200</v>
       </c>
-      <c r="E15">
+      <c r="E16" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="12">
+        <v>64</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12">
         <v>2016</v>
       </c>
-      <c r="F15">
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="13">
+        <v>1</v>
+      </c>
+      <c r="O16" s="12">
         <v>2020</v>
       </c>
-      <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="P16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2608333333333333</v>
+      </c>
+      <c r="C17">
+        <v>3913</v>
+      </c>
+      <c r="D17">
+        <v>1200</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
         <v>61</v>
       </c>
-      <c r="J15">
+      <c r="H17">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>3.2608333333333333</v>
-      </c>
-      <c r="C16">
-        <v>3913</v>
-      </c>
-      <c r="D16">
-        <v>1200</v>
-      </c>
-      <c r="E16">
+      <c r="J17">
         <v>2015</v>
       </c>
-      <c r="F16">
+      <c r="O17">
         <v>2020</v>
       </c>
-      <c r="H16" t="s">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>5.504666666666667</v>
+      </c>
+      <c r="C18">
+        <v>8257</v>
+      </c>
+      <c r="D18">
+        <v>1500</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
         <v>63</v>
       </c>
-      <c r="I16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16">
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="J18">
+        <v>2019</v>
+      </c>
+      <c r="N18" s="6">
+        <v>4</v>
+      </c>
+      <c r="O18">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>4.4584967320261439</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>13643</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>3060</v>
       </c>
-      <c r="E17">
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19">
+        <v>64</v>
+      </c>
+      <c r="J19">
         <v>2009</v>
       </c>
-      <c r="F17">
+      <c r="N19" s="6">
+        <v>24</v>
+      </c>
+      <c r="O19">
         <v>2020</v>
       </c>
-      <c r="G17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" t="s">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="1">
+        <f>C20/D20</f>
+        <v>6.3620000000000001</v>
+      </c>
+      <c r="C20">
+        <v>19086</v>
+      </c>
+      <c r="D20">
+        <v>3000</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s">
         <v>64</v>
       </c>
-      <c r="I17" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17">
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="1">
-        <f>C18/D18</f>
-        <v>6.3620000000000001</v>
-      </c>
-      <c r="C18">
-        <v>19086</v>
-      </c>
-      <c r="D18">
-        <v>3000</v>
-      </c>
-      <c r="E18">
+      <c r="J20">
         <v>2013</v>
       </c>
-      <c r="F18">
+      <c r="N20" s="6">
+        <v>16</v>
+      </c>
+      <c r="O20">
         <v>2024</v>
       </c>
-      <c r="G18" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" t="s">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" ref="B21:B25" si="1">C21/D21</f>
+        <v>6.4378787878787875</v>
+      </c>
+      <c r="C21">
+        <v>21245</v>
+      </c>
+      <c r="D21">
+        <v>3300</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
         <v>64</v>
       </c>
-      <c r="I18" t="s">
+      <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="J18">
+      <c r="H21">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
-        <f t="shared" ref="B19:B23" si="1">C19/D19</f>
-        <v>6.4378787878787875</v>
-      </c>
-      <c r="C19">
-        <v>21245</v>
-      </c>
-      <c r="D19">
-        <v>3300</v>
-      </c>
-      <c r="E19">
+      <c r="J21">
         <v>2012</v>
       </c>
-      <c r="F19">
+      <c r="N21" s="6">
+        <v>16</v>
+      </c>
+      <c r="O21">
         <v>2020</v>
       </c>
-      <c r="G19" t="s">
-        <v>83</v>
-      </c>
-      <c r="H19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" t="s">
-        <v>66</v>
-      </c>
-      <c r="J19">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B22" s="1">
         <f t="shared" si="1"/>
         <v>6.4969945355191259</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>23779</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>3660</v>
       </c>
-      <c r="E20">
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22">
+        <v>64</v>
+      </c>
+      <c r="J22">
         <v>2015</v>
       </c>
-      <c r="F20">
+      <c r="N22" s="6">
+        <v>24</v>
+      </c>
+      <c r="O22">
         <v>2020</v>
       </c>
-      <c r="G20" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B23" s="1">
         <f t="shared" si="1"/>
         <v>7.2350710900473931</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>30532</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>4220</v>
       </c>
-      <c r="E21">
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23">
+        <v>64</v>
+      </c>
+      <c r="J23">
         <v>2020</v>
       </c>
-      <c r="F21">
+      <c r="N23" s="6">
+        <v>48</v>
+      </c>
+      <c r="O23">
         <v>2021</v>
       </c>
-      <c r="G21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B24" s="1">
         <f t="shared" si="1"/>
         <v>8.4960869565217383</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>39082</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>4600</v>
       </c>
-      <c r="E22">
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24">
+        <v>64</v>
+      </c>
+      <c r="J24">
         <v>2023</v>
       </c>
-      <c r="F22">
+      <c r="N24" s="6">
+        <v>64</v>
+      </c>
+      <c r="O24">
         <v>2024</v>
       </c>
-      <c r="G22" t="s">
-        <v>74</v>
-      </c>
-      <c r="H22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" t="s">
-        <v>75</v>
-      </c>
-      <c r="J22">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B25" s="1">
         <f t="shared" si="1"/>
         <v>9.9118750000000002</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>31718</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>3200</v>
       </c>
-      <c r="E23">
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25">
+        <v>64</v>
+      </c>
+      <c r="J25">
         <v>2020</v>
       </c>
-      <c r="F23" s="3">
+      <c r="N25" s="6">
+        <v>16</v>
+      </c>
+      <c r="O25" s="3">
         <v>2023</v>
       </c>
-      <c r="G23" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" t="s">
-        <v>71</v>
-      </c>
-      <c r="I23" t="s">
-        <v>70</v>
-      </c>
-      <c r="J23">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1" xr:uid="{14E13CF2-D12C-470D-B931-64AFEE59DDEB}"/>
+    <hyperlink ref="A31" r:id="rId1" xr:uid="{14E13CF2-D12C-470D-B931-64AFEE59DDEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1387,7 +1662,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -1677,7 +1952,7 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>

</xml_diff>